<commit_message>
added all logitech warranty skus
</commit_message>
<xml_diff>
--- a/MASTER AV PRICING.xlsx
+++ b/MASTER AV PRICING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruce/Documents/GitHub/av_equipment_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01631AAE-48FB-484C-BCBA-EFD500A6D94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E287F6E-2194-5A4C-96C0-BC3B87A19E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10500" yWindow="5560" windowWidth="36000" windowHeight="21280" xr2:uid="{96C77E46-4F69-4449-AA02-281EC9495813}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9397" uniqueCount="4656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9629" uniqueCount="4761">
   <si>
     <t>PART</t>
   </si>
@@ -14149,6 +14149,321 @@
   </si>
   <si>
     <t>3 year extended warranty for standalone Logitech TAP IP (952-000085 or 952-000088). TAP IP serial number is required with order.</t>
+  </si>
+  <si>
+    <t>994-000093</t>
+  </si>
+  <si>
+    <t>994-000177</t>
+  </si>
+  <si>
+    <t>994-000108</t>
+  </si>
+  <si>
+    <t>994-000144</t>
+  </si>
+  <si>
+    <t>994-000173</t>
+  </si>
+  <si>
+    <t>994-000252</t>
+  </si>
+  <si>
+    <t>994-000192</t>
+  </si>
+  <si>
+    <t>994-000109</t>
+  </si>
+  <si>
+    <t>994-000143</t>
+  </si>
+  <si>
+    <t>994-000174</t>
+  </si>
+  <si>
+    <t>994-000110</t>
+  </si>
+  <si>
+    <t>994-000240</t>
+  </si>
+  <si>
+    <t>994-000222</t>
+  </si>
+  <si>
+    <t>994-000098</t>
+  </si>
+  <si>
+    <t>994-000353</t>
+  </si>
+  <si>
+    <t>994-000137</t>
+  </si>
+  <si>
+    <t>994-000138</t>
+  </si>
+  <si>
+    <t>994-000248</t>
+  </si>
+  <si>
+    <t>994-000100</t>
+  </si>
+  <si>
+    <t>994-000101</t>
+  </si>
+  <si>
+    <t>994-000107</t>
+  </si>
+  <si>
+    <t>994-000139</t>
+  </si>
+  <si>
+    <t>994-000147</t>
+  </si>
+  <si>
+    <t>994-000125</t>
+  </si>
+  <si>
+    <t>994-000150</t>
+  </si>
+  <si>
+    <t>994-000151</t>
+  </si>
+  <si>
+    <t>994-000258</t>
+  </si>
+  <si>
+    <t>994-000167</t>
+  </si>
+  <si>
+    <t>Base bundle with Tap, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Base bundle with Tap IP &amp; RoomMate, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Small room bundle with MeetUp &amp; Tap, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Small room bundle with Rally Bar Mini &amp; Tap, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Small room bundle with Rally Bar Mini &amp; Tap IP, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Bundle with Rally Bar Huddle &amp; Tap IP, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Huddle room bundle with MeetUp, RoomMate &amp; Tap IP, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Medium room bundle with Rally &amp; Tap, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Medium room bundle with Rally Bar &amp; Tap, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Medium room bundle with Rally Bar &amp; Tap IP, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Large room bundle with Rally Plus &amp; Tap, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Sight, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Logi Dock Focus Room Kit, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>MeetUp, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>MeetUp + Mic, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>MeetUp 2, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally Bar, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally Bar Mini, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally Bar Huddle, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally Plus, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally Camera, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>RoomMate, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Scribe, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Swytch, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Tap IP, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Tap Scheduler, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Logi Dock Flex, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Logi Dock, 1-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>994-000153</t>
+  </si>
+  <si>
+    <t>994-000160</t>
+  </si>
+  <si>
+    <t>994-000172</t>
+  </si>
+  <si>
+    <t>994-000175</t>
+  </si>
+  <si>
+    <t>994-000193</t>
+  </si>
+  <si>
+    <t>994-000161</t>
+  </si>
+  <si>
+    <t>994-000171</t>
+  </si>
+  <si>
+    <t>994-000176</t>
+  </si>
+  <si>
+    <t>994-000162</t>
+  </si>
+  <si>
+    <t>994-000239</t>
+  </si>
+  <si>
+    <t>994-000223</t>
+  </si>
+  <si>
+    <t>994-000154</t>
+  </si>
+  <si>
+    <t>994-000352</t>
+  </si>
+  <si>
+    <t>994-000249</t>
+  </si>
+  <si>
+    <t>994-000155</t>
+  </si>
+  <si>
+    <t>994-000164</t>
+  </si>
+  <si>
+    <t>994-000165</t>
+  </si>
+  <si>
+    <t>994-000259</t>
+  </si>
+  <si>
+    <t>994-000166</t>
+  </si>
+  <si>
+    <t>Base bundle with Tap, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Base bundle with Tap IP &amp; RoomMate, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Small room bundle with MeetUp &amp; Tap, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Small room bundle with Rally Bar Mini &amp; Tap, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Small room bundle with Rally Bar Mini &amp; Tap IP, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Bundle with Rally Bar Huddle &amp; Tap IP, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Huddle room bundle with MeetUp, RoomMate &amp; Tap IP, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Medium room bundle with Rally &amp; Tap, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Medium room bundle with Rally Bar &amp; Tap, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Medium room bundle with Rally Bar &amp; Tap IP, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Large room bundle with Rally Plus &amp; Tap, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Sight, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Logi Dock Focus Room Kit, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>MeetUp, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>MeetUp + Mic, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>MeetUp 2, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally Bar, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally Bar Mini, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally Bar Huddle, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally Plus, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Rally Camera, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>RoomMate, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Scribe, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Swytch, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Tap IP, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Tap Scheduler, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Logi Dock Flex, 3-Year Extended Warranty, requires device serial number is required with order.</t>
+  </si>
+  <si>
+    <t>Logi Dock, 3-Year Extended Warranty, requires device serial number is required with order.</t>
   </si>
 </sst>
 </file>
@@ -14580,8 +14895,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD929915-576A-754E-997F-E4D1009117F2}" name="DEVICES" displayName="DEVICES" ref="A1:G2350" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:G2350" xr:uid="{CD929915-576A-754E-997F-E4D1009117F2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD929915-576A-754E-997F-E4D1009117F2}" name="DEVICES" displayName="DEVICES" ref="A1:G2408" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:G2408" xr:uid="{CD929915-576A-754E-997F-E4D1009117F2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G2343">
     <sortCondition ref="D1:D2343"/>
   </sortState>
@@ -14897,10 +15212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6A0869-A5FD-BB4C-AF5E-D022C2EF8E42}">
-  <dimension ref="A1:G2350"/>
+  <dimension ref="A1:G2408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2317" workbookViewId="0">
-      <selection activeCell="C2352" sqref="C2352"/>
+    <sheetView tabSelected="1" topLeftCell="A2364" workbookViewId="0">
+      <selection activeCell="H2390" sqref="H2390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -57243,6 +57558,1166 @@
       </c>
       <c r="F2350" s="28"/>
       <c r="G2350" s="48"/>
+    </row>
+    <row r="2351" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2351" t="str">
+        <f>_xlfn.CONCAT(B2351,D2351,E2351)</f>
+        <v>WARRANTY-LOGITECH994-000093</v>
+      </c>
+      <c r="B2351" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2351" s="26" t="s">
+        <v>4684</v>
+      </c>
+      <c r="D2351" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2351" t="s">
+        <v>4656</v>
+      </c>
+      <c r="F2351" s="28"/>
+      <c r="G2351" s="48"/>
+    </row>
+    <row r="2352" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2352" t="str">
+        <f t="shared" ref="A2352:A2379" si="1">_xlfn.CONCAT(B2352,D2352,E2352)</f>
+        <v>WARRANTY-LOGITECH994-000177</v>
+      </c>
+      <c r="B2352" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2352" s="26" t="s">
+        <v>4685</v>
+      </c>
+      <c r="D2352" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2352" t="s">
+        <v>4657</v>
+      </c>
+      <c r="F2352" s="28"/>
+      <c r="G2352" s="28"/>
+    </row>
+    <row r="2353" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2353" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000108</v>
+      </c>
+      <c r="B2353" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2353" s="26" t="s">
+        <v>4686</v>
+      </c>
+      <c r="D2353" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2353" t="s">
+        <v>4658</v>
+      </c>
+      <c r="F2353" s="28"/>
+      <c r="G2353" s="28"/>
+    </row>
+    <row r="2354" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2354" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000144</v>
+      </c>
+      <c r="B2354" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2354" s="26" t="s">
+        <v>4687</v>
+      </c>
+      <c r="D2354" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2354" t="s">
+        <v>4659</v>
+      </c>
+      <c r="F2354" s="28"/>
+      <c r="G2354" s="28"/>
+    </row>
+    <row r="2355" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2355" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000173</v>
+      </c>
+      <c r="B2355" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2355" s="26" t="s">
+        <v>4688</v>
+      </c>
+      <c r="D2355" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2355" t="s">
+        <v>4660</v>
+      </c>
+      <c r="F2355" s="28"/>
+      <c r="G2355" s="28"/>
+    </row>
+    <row r="2356" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2356" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000252</v>
+      </c>
+      <c r="B2356" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2356" s="26" t="s">
+        <v>4689</v>
+      </c>
+      <c r="D2356" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2356" t="s">
+        <v>4661</v>
+      </c>
+      <c r="F2356" s="28"/>
+      <c r="G2356" s="28"/>
+    </row>
+    <row r="2357" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2357" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000192</v>
+      </c>
+      <c r="B2357" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2357" s="26" t="s">
+        <v>4690</v>
+      </c>
+      <c r="D2357" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2357" t="s">
+        <v>4662</v>
+      </c>
+      <c r="F2357" s="28"/>
+      <c r="G2357" s="28"/>
+    </row>
+    <row r="2358" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2358" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000109</v>
+      </c>
+      <c r="B2358" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2358" s="26" t="s">
+        <v>4691</v>
+      </c>
+      <c r="D2358" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2358" t="s">
+        <v>4663</v>
+      </c>
+      <c r="F2358" s="28"/>
+      <c r="G2358" s="28"/>
+    </row>
+    <row r="2359" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2359" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000143</v>
+      </c>
+      <c r="B2359" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2359" s="26" t="s">
+        <v>4692</v>
+      </c>
+      <c r="D2359" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2359" t="s">
+        <v>4664</v>
+      </c>
+      <c r="F2359" s="28"/>
+      <c r="G2359" s="28"/>
+    </row>
+    <row r="2360" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2360" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000174</v>
+      </c>
+      <c r="B2360" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2360" s="26" t="s">
+        <v>4693</v>
+      </c>
+      <c r="D2360" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2360" t="s">
+        <v>4665</v>
+      </c>
+      <c r="F2360" s="28"/>
+      <c r="G2360" s="28"/>
+    </row>
+    <row r="2361" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2361" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000110</v>
+      </c>
+      <c r="B2361" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2361" s="26" t="s">
+        <v>4694</v>
+      </c>
+      <c r="D2361" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2361" t="s">
+        <v>4666</v>
+      </c>
+      <c r="F2361" s="28"/>
+      <c r="G2361" s="28"/>
+    </row>
+    <row r="2362" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2362" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000240</v>
+      </c>
+      <c r="B2362" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2362" s="26" t="s">
+        <v>4695</v>
+      </c>
+      <c r="D2362" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2362" t="s">
+        <v>4667</v>
+      </c>
+      <c r="F2362" s="28"/>
+      <c r="G2362" s="28"/>
+    </row>
+    <row r="2363" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2363" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000222</v>
+      </c>
+      <c r="B2363" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2363" s="26" t="s">
+        <v>4696</v>
+      </c>
+      <c r="D2363" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2363" t="s">
+        <v>4668</v>
+      </c>
+      <c r="F2363" s="28"/>
+      <c r="G2363" s="28"/>
+    </row>
+    <row r="2364" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2364" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000098</v>
+      </c>
+      <c r="B2364" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2364" s="26" t="s">
+        <v>4697</v>
+      </c>
+      <c r="D2364" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2364" t="s">
+        <v>4669</v>
+      </c>
+      <c r="F2364" s="28"/>
+      <c r="G2364" s="28"/>
+    </row>
+    <row r="2365" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2365" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000098</v>
+      </c>
+      <c r="B2365" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2365" s="26" t="s">
+        <v>4698</v>
+      </c>
+      <c r="D2365" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2365" t="s">
+        <v>4669</v>
+      </c>
+      <c r="F2365" s="28"/>
+      <c r="G2365" s="28"/>
+    </row>
+    <row r="2366" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2366" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000353</v>
+      </c>
+      <c r="B2366" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2366" s="26" t="s">
+        <v>4699</v>
+      </c>
+      <c r="D2366" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2366" t="s">
+        <v>4670</v>
+      </c>
+      <c r="F2366" s="28"/>
+      <c r="G2366" s="28"/>
+    </row>
+    <row r="2367" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2367" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000137</v>
+      </c>
+      <c r="B2367" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2367" s="26" t="s">
+        <v>4700</v>
+      </c>
+      <c r="D2367" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2367" t="s">
+        <v>4671</v>
+      </c>
+      <c r="F2367" s="28"/>
+      <c r="G2367" s="28"/>
+    </row>
+    <row r="2368" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2368" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000138</v>
+      </c>
+      <c r="B2368" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2368" s="26" t="s">
+        <v>4701</v>
+      </c>
+      <c r="D2368" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2368" t="s">
+        <v>4672</v>
+      </c>
+      <c r="F2368" s="28"/>
+      <c r="G2368" s="28"/>
+    </row>
+    <row r="2369" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2369" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000248</v>
+      </c>
+      <c r="B2369" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2369" s="26" t="s">
+        <v>4702</v>
+      </c>
+      <c r="D2369" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2369" t="s">
+        <v>4673</v>
+      </c>
+      <c r="F2369" s="28"/>
+      <c r="G2369" s="28"/>
+    </row>
+    <row r="2370" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2370" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000100</v>
+      </c>
+      <c r="B2370" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2370" s="26" t="s">
+        <v>4703</v>
+      </c>
+      <c r="D2370" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2370" t="s">
+        <v>4674</v>
+      </c>
+      <c r="F2370" s="28"/>
+      <c r="G2370" s="28"/>
+    </row>
+    <row r="2371" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2371" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000101</v>
+      </c>
+      <c r="B2371" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2371" s="26" t="s">
+        <v>4704</v>
+      </c>
+      <c r="D2371" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2371" t="s">
+        <v>4675</v>
+      </c>
+      <c r="F2371" s="28"/>
+      <c r="G2371" s="28"/>
+    </row>
+    <row r="2372" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2372" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000107</v>
+      </c>
+      <c r="B2372" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2372" s="26" t="s">
+        <v>4705</v>
+      </c>
+      <c r="D2372" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2372" t="s">
+        <v>4676</v>
+      </c>
+      <c r="F2372" s="28"/>
+      <c r="G2372" s="28"/>
+    </row>
+    <row r="2373" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2373" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000139</v>
+      </c>
+      <c r="B2373" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2373" s="26" t="s">
+        <v>4706</v>
+      </c>
+      <c r="D2373" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2373" t="s">
+        <v>4677</v>
+      </c>
+      <c r="F2373" s="28"/>
+      <c r="G2373" s="28"/>
+    </row>
+    <row r="2374" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2374" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000147</v>
+      </c>
+      <c r="B2374" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2374" s="26" t="s">
+        <v>4707</v>
+      </c>
+      <c r="D2374" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2374" t="s">
+        <v>4678</v>
+      </c>
+      <c r="F2374" s="28"/>
+      <c r="G2374" s="28"/>
+    </row>
+    <row r="2375" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2375" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000125</v>
+      </c>
+      <c r="B2375" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2375" s="26" t="s">
+        <v>4708</v>
+      </c>
+      <c r="D2375" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2375" t="s">
+        <v>4679</v>
+      </c>
+      <c r="F2375" s="28"/>
+      <c r="G2375" s="28"/>
+    </row>
+    <row r="2376" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2376" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000150</v>
+      </c>
+      <c r="B2376" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2376" s="26" t="s">
+        <v>4709</v>
+      </c>
+      <c r="D2376" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2376" t="s">
+        <v>4680</v>
+      </c>
+      <c r="F2376" s="28"/>
+      <c r="G2376" s="28"/>
+    </row>
+    <row r="2377" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2377" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000151</v>
+      </c>
+      <c r="B2377" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2377" s="26" t="s">
+        <v>4710</v>
+      </c>
+      <c r="D2377" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2377" t="s">
+        <v>4681</v>
+      </c>
+      <c r="F2377" s="28"/>
+      <c r="G2377" s="28"/>
+    </row>
+    <row r="2378" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2378" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000258</v>
+      </c>
+      <c r="B2378" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2378" s="26" t="s">
+        <v>4711</v>
+      </c>
+      <c r="D2378" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2378" t="s">
+        <v>4682</v>
+      </c>
+      <c r="F2378" s="28"/>
+      <c r="G2378" s="28"/>
+    </row>
+    <row r="2379" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2379" t="str">
+        <f t="shared" si="1"/>
+        <v>WARRANTY-LOGITECH994-000167</v>
+      </c>
+      <c r="B2379" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2379" s="26" t="s">
+        <v>4712</v>
+      </c>
+      <c r="D2379" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2379" t="s">
+        <v>4683</v>
+      </c>
+      <c r="F2379" s="28"/>
+      <c r="G2379" s="28"/>
+    </row>
+    <row r="2380" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2380" s="30" t="str">
+        <f>_xlfn.CONCAT(B2380,D2380,E2380)</f>
+        <v>WARRANTY-LOGITECH994-000153</v>
+      </c>
+      <c r="B2380" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2380" s="46" t="s">
+        <v>4732</v>
+      </c>
+      <c r="D2380" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2380" t="s">
+        <v>4713</v>
+      </c>
+      <c r="F2380" s="48"/>
+      <c r="G2380" s="48"/>
+    </row>
+    <row r="2381" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2381" t="str">
+        <f t="shared" ref="A2381:A2408" si="2">_xlfn.CONCAT(B2381,D2381,E2381)</f>
+        <v>WARRANTY-LOGITECH994-000178</v>
+      </c>
+      <c r="B2381" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2381" s="26" t="s">
+        <v>4733</v>
+      </c>
+      <c r="D2381" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2381" t="s">
+        <v>4624</v>
+      </c>
+      <c r="F2381" s="28"/>
+      <c r="G2381" s="28"/>
+    </row>
+    <row r="2382" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2382" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000160</v>
+      </c>
+      <c r="B2382" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2382" s="26" t="s">
+        <v>4734</v>
+      </c>
+      <c r="D2382" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2382" t="s">
+        <v>4714</v>
+      </c>
+      <c r="F2382" s="28"/>
+      <c r="G2382" s="28"/>
+    </row>
+    <row r="2383" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2383" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000172</v>
+      </c>
+      <c r="B2383" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2383" s="26" t="s">
+        <v>4735</v>
+      </c>
+      <c r="D2383" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2383" t="s">
+        <v>4715</v>
+      </c>
+      <c r="F2383" s="28"/>
+      <c r="G2383" s="28"/>
+    </row>
+    <row r="2384" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2384" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000175</v>
+      </c>
+      <c r="B2384" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2384" s="26" t="s">
+        <v>4736</v>
+      </c>
+      <c r="D2384" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2384" t="s">
+        <v>4716</v>
+      </c>
+      <c r="F2384" s="28"/>
+      <c r="G2384" s="28"/>
+    </row>
+    <row r="2385" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2385" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000253</v>
+      </c>
+      <c r="B2385" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2385" s="26" t="s">
+        <v>4737</v>
+      </c>
+      <c r="D2385" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2385" t="s">
+        <v>4650</v>
+      </c>
+      <c r="F2385" s="28"/>
+      <c r="G2385" s="28"/>
+    </row>
+    <row r="2386" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2386" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000193</v>
+      </c>
+      <c r="B2386" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2386" s="26" t="s">
+        <v>4738</v>
+      </c>
+      <c r="D2386" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2386" t="s">
+        <v>4717</v>
+      </c>
+      <c r="F2386" s="28"/>
+      <c r="G2386" s="28"/>
+    </row>
+    <row r="2387" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2387" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000161</v>
+      </c>
+      <c r="B2387" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2387" s="26" t="s">
+        <v>4739</v>
+      </c>
+      <c r="D2387" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2387" t="s">
+        <v>4718</v>
+      </c>
+      <c r="F2387" s="28"/>
+      <c r="G2387" s="28"/>
+    </row>
+    <row r="2388" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2388" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000171</v>
+      </c>
+      <c r="B2388" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2388" s="26" t="s">
+        <v>4740</v>
+      </c>
+      <c r="D2388" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2388" t="s">
+        <v>4719</v>
+      </c>
+      <c r="F2388" s="28"/>
+      <c r="G2388" s="28"/>
+    </row>
+    <row r="2389" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2389" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000176</v>
+      </c>
+      <c r="B2389" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2389" s="26" t="s">
+        <v>4741</v>
+      </c>
+      <c r="D2389" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2389" t="s">
+        <v>4720</v>
+      </c>
+      <c r="F2389" s="28"/>
+      <c r="G2389" s="28"/>
+    </row>
+    <row r="2390" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2390" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000162</v>
+      </c>
+      <c r="B2390" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2390" s="26" t="s">
+        <v>4742</v>
+      </c>
+      <c r="D2390" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2390" t="s">
+        <v>4721</v>
+      </c>
+      <c r="F2390" s="28"/>
+      <c r="G2390" s="28"/>
+    </row>
+    <row r="2391" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2391" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000239</v>
+      </c>
+      <c r="B2391" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2391" s="26" t="s">
+        <v>4743</v>
+      </c>
+      <c r="D2391" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2391" t="s">
+        <v>4722</v>
+      </c>
+      <c r="F2391" s="28"/>
+      <c r="G2391" s="28"/>
+    </row>
+    <row r="2392" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2392" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000223</v>
+      </c>
+      <c r="B2392" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2392" s="26" t="s">
+        <v>4744</v>
+      </c>
+      <c r="D2392" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2392" t="s">
+        <v>4723</v>
+      </c>
+      <c r="F2392" s="28"/>
+      <c r="G2392" s="28"/>
+    </row>
+    <row r="2393" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2393" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000154</v>
+      </c>
+      <c r="B2393" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2393" s="26" t="s">
+        <v>4745</v>
+      </c>
+      <c r="D2393" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2393" t="s">
+        <v>4724</v>
+      </c>
+      <c r="F2393" s="28"/>
+      <c r="G2393" s="28"/>
+    </row>
+    <row r="2394" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2394" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000154</v>
+      </c>
+      <c r="B2394" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2394" s="26" t="s">
+        <v>4746</v>
+      </c>
+      <c r="D2394" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2394" t="s">
+        <v>4724</v>
+      </c>
+      <c r="F2394" s="28"/>
+      <c r="G2394" s="28"/>
+    </row>
+    <row r="2395" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2395" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000352</v>
+      </c>
+      <c r="B2395" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2395" s="26" t="s">
+        <v>4747</v>
+      </c>
+      <c r="D2395" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2395" t="s">
+        <v>4725</v>
+      </c>
+      <c r="F2395" s="28"/>
+      <c r="G2395" s="28"/>
+    </row>
+    <row r="2396" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2396" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000168</v>
+      </c>
+      <c r="B2396" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2396" s="26" t="s">
+        <v>4748</v>
+      </c>
+      <c r="D2396" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2396" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F2396" s="28"/>
+      <c r="G2396" s="28"/>
+    </row>
+    <row r="2397" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2397" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000169</v>
+      </c>
+      <c r="B2397" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2397" s="26" t="s">
+        <v>4749</v>
+      </c>
+      <c r="D2397" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2397" t="s">
+        <v>1298</v>
+      </c>
+      <c r="F2397" s="28"/>
+      <c r="G2397" s="28"/>
+    </row>
+    <row r="2398" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2398" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000249</v>
+      </c>
+      <c r="B2398" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2398" s="26" t="s">
+        <v>4750</v>
+      </c>
+      <c r="D2398" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2398" t="s">
+        <v>4726</v>
+      </c>
+      <c r="F2398" s="28"/>
+      <c r="G2398" s="28"/>
+    </row>
+    <row r="2399" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2399" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000155</v>
+      </c>
+      <c r="B2399" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2399" s="26" t="s">
+        <v>4751</v>
+      </c>
+      <c r="D2399" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2399" t="s">
+        <v>4727</v>
+      </c>
+      <c r="F2399" s="28"/>
+      <c r="G2399" s="28"/>
+    </row>
+    <row r="2400" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2400" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000156</v>
+      </c>
+      <c r="B2400" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2400" s="26" t="s">
+        <v>4752</v>
+      </c>
+      <c r="D2400" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2400" t="s">
+        <v>1164</v>
+      </c>
+      <c r="F2400" s="28"/>
+      <c r="G2400" s="28"/>
+    </row>
+    <row r="2401" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2401" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000157</v>
+      </c>
+      <c r="B2401" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2401" s="26" t="s">
+        <v>4753</v>
+      </c>
+      <c r="D2401" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2401" t="s">
+        <v>1108</v>
+      </c>
+      <c r="F2401" s="28"/>
+      <c r="G2401" s="28"/>
+    </row>
+    <row r="2402" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2402" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000170</v>
+      </c>
+      <c r="B2402" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2402" s="26" t="s">
+        <v>4754</v>
+      </c>
+      <c r="D2402" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2402" t="s">
+        <v>4622</v>
+      </c>
+      <c r="F2402" s="28"/>
+      <c r="G2402" s="28"/>
+    </row>
+    <row r="2403" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2403" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000164</v>
+      </c>
+      <c r="B2403" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2403" s="26" t="s">
+        <v>4755</v>
+      </c>
+      <c r="D2403" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2403" t="s">
+        <v>4728</v>
+      </c>
+      <c r="F2403" s="28"/>
+      <c r="G2403" s="28"/>
+    </row>
+    <row r="2404" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2404" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000165</v>
+      </c>
+      <c r="B2404" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2404" s="26" t="s">
+        <v>4756</v>
+      </c>
+      <c r="D2404" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2404" t="s">
+        <v>4729</v>
+      </c>
+      <c r="F2404" s="28"/>
+      <c r="G2404" s="28"/>
+    </row>
+    <row r="2405" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2405" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000159</v>
+      </c>
+      <c r="B2405" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2405" s="26" t="s">
+        <v>4757</v>
+      </c>
+      <c r="D2405" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2405" t="s">
+        <v>4654</v>
+      </c>
+      <c r="F2405" s="28"/>
+      <c r="G2405" s="28"/>
+    </row>
+    <row r="2406" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2406" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000163</v>
+      </c>
+      <c r="B2406" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2406" s="26" t="s">
+        <v>4758</v>
+      </c>
+      <c r="D2406" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2406" t="s">
+        <v>4652</v>
+      </c>
+      <c r="F2406" s="28"/>
+      <c r="G2406" s="28"/>
+    </row>
+    <row r="2407" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2407" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000259</v>
+      </c>
+      <c r="B2407" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2407" s="26" t="s">
+        <v>4759</v>
+      </c>
+      <c r="D2407" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2407" t="s">
+        <v>4730</v>
+      </c>
+      <c r="F2407" s="28"/>
+      <c r="G2407" s="28"/>
+    </row>
+    <row r="2408" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2408" t="str">
+        <f t="shared" si="2"/>
+        <v>WARRANTY-LOGITECH994-000166</v>
+      </c>
+      <c r="B2408" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2408" s="26" t="s">
+        <v>4760</v>
+      </c>
+      <c r="D2408" s="47" t="s">
+        <v>4607</v>
+      </c>
+      <c r="E2408" t="s">
+        <v>4731</v>
+      </c>
+      <c r="F2408" s="28"/>
+      <c r="G2408" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>

</xml_diff>